<commit_message>
We now have the correct code for the playwright of this new project 2, tha affiliate pnl
</commit_message>
<xml_diff>
--- a/a1_master_database_gf.xlsx
+++ b/a1_master_database_gf.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18182" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18236" uniqueCount="780">
   <si>
     <t>Class</t>
   </si>
@@ -2346,6 +2346,15 @@
   <si>
     <t>2025-06-30 23:30:00</t>
   </si>
+  <si>
+    <t>2025-07-01 09:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-01 09:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-01 10:00:00</t>
+  </si>
 </sst>
 </file>
 
@@ -2702,7 +2711,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6060"/>
+  <dimension ref="A1:E6078"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -105728,6 +105737,312 @@
         <v>776</v>
       </c>
     </row>
+    <row r="6061" spans="1:5">
+      <c r="A6061" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6061" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6061">
+        <v>30</v>
+      </c>
+      <c r="D6061">
+        <v>12</v>
+      </c>
+      <c r="E6061" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="6062" spans="1:5">
+      <c r="A6062" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6062" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6062">
+        <v>14.29</v>
+      </c>
+      <c r="D6062">
+        <v>14</v>
+      </c>
+      <c r="E6062" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="6063" spans="1:5">
+      <c r="A6063" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6063" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6063">
+        <v>0</v>
+      </c>
+      <c r="D6063">
+        <v>3</v>
+      </c>
+      <c r="E6063" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="6064" spans="1:5">
+      <c r="A6064" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6064" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6064">
+        <v>100</v>
+      </c>
+      <c r="D6064">
+        <v>4</v>
+      </c>
+      <c r="E6064" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="6065" spans="1:5">
+      <c r="A6065" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6065" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6065">
+        <v>0</v>
+      </c>
+      <c r="D6065">
+        <v>0</v>
+      </c>
+      <c r="E6065" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="6066" spans="1:5">
+      <c r="A6066" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6066" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6066">
+        <v>0</v>
+      </c>
+      <c r="D6066">
+        <v>0</v>
+      </c>
+      <c r="E6066" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="6067" spans="1:5">
+      <c r="A6067" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6067" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6067">
+        <v>30</v>
+      </c>
+      <c r="D6067">
+        <v>12</v>
+      </c>
+      <c r="E6067" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="6068" spans="1:5">
+      <c r="A6068" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6068" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6068">
+        <v>9.09</v>
+      </c>
+      <c r="D6068">
+        <v>22</v>
+      </c>
+      <c r="E6068" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="6069" spans="1:5">
+      <c r="A6069" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6069" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6069">
+        <v>0</v>
+      </c>
+      <c r="D6069">
+        <v>4</v>
+      </c>
+      <c r="E6069" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="6070" spans="1:5">
+      <c r="A6070" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6070" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6070">
+        <v>66.67</v>
+      </c>
+      <c r="D6070">
+        <v>5</v>
+      </c>
+      <c r="E6070" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="6071" spans="1:5">
+      <c r="A6071" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6071" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6071">
+        <v>0</v>
+      </c>
+      <c r="D6071">
+        <v>1</v>
+      </c>
+      <c r="E6071" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="6072" spans="1:5">
+      <c r="A6072" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6072" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6072">
+        <v>0</v>
+      </c>
+      <c r="D6072">
+        <v>2</v>
+      </c>
+      <c r="E6072" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="6073" spans="1:5">
+      <c r="A6073" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6073" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6073">
+        <v>33.33</v>
+      </c>
+      <c r="D6073">
+        <v>17</v>
+      </c>
+      <c r="E6073" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="6074" spans="1:5">
+      <c r="A6074" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6074" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6074">
+        <v>10</v>
+      </c>
+      <c r="D6074">
+        <v>30</v>
+      </c>
+      <c r="E6074" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="6075" spans="1:5">
+      <c r="A6075" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6075" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6075">
+        <v>16.67</v>
+      </c>
+      <c r="D6075">
+        <v>7</v>
+      </c>
+      <c r="E6075" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="6076" spans="1:5">
+      <c r="A6076" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6076" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6076">
+        <v>50</v>
+      </c>
+      <c r="D6076">
+        <v>6</v>
+      </c>
+      <c r="E6076" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="6077" spans="1:5">
+      <c r="A6077" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6077" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6077">
+        <v>50</v>
+      </c>
+      <c r="D6077">
+        <v>3</v>
+      </c>
+      <c r="E6077" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="6078" spans="1:5">
+      <c r="A6078" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6078" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6078">
+        <v>50</v>
+      </c>
+      <c r="D6078">
+        <v>2</v>
+      </c>
+      <c r="E6078" t="s">
+        <v>779</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>